<commit_message>
removed spaces from ecogroup names
</commit_message>
<xml_diff>
--- a/cichlid_sr_sequencing/SampleDatabase.xlsx
+++ b/cichlid_sr_sequencing/SampleDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmnike/Desktop/VCF_Excel_Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFD3CAC-3F1E-424A-B922-7970E5BD8417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED97341-4B40-A041-A2E2-9DD9A20645AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDatabase" sheetId="1" r:id="rId1"/>
@@ -57817,7 +57817,7 @@
   <dimension ref="A1:P523"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57834,7 +57834,7 @@
     <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="67.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
     <col min="14" max="14" width="40.33203125" customWidth="1"/>
     <col min="15" max="15" width="29.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="31.83203125" bestFit="1" customWidth="1"/>
@@ -58123,7 +58123,7 @@
         <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="P6" s="8">
         <v>157</v>
@@ -58170,7 +58170,7 @@
         <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
       <c r="P7" s="8">
         <v>27</v>
@@ -58397,7 +58397,7 @@
         <v>74</v>
       </c>
       <c r="M12" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -58438,7 +58438,7 @@
         <v>74</v>
       </c>
       <c r="M13" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -58891,7 +58891,7 @@
         <v>132</v>
       </c>
       <c r="M24" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
@@ -59506,7 +59506,7 @@
         <v>196</v>
       </c>
       <c r="M39" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -59547,7 +59547,7 @@
         <v>196</v>
       </c>
       <c r="M40" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -59588,7 +59588,7 @@
         <v>196</v>
       </c>
       <c r="M41" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -59629,7 +59629,7 @@
         <v>196</v>
       </c>
       <c r="M42" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
@@ -59670,7 +59670,7 @@
         <v>196</v>
       </c>
       <c r="M43" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
@@ -59711,7 +59711,7 @@
         <v>196</v>
       </c>
       <c r="M44" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
@@ -59752,7 +59752,7 @@
         <v>221</v>
       </c>
       <c r="M45" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
@@ -59793,7 +59793,7 @@
         <v>221</v>
       </c>
       <c r="M46" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
@@ -59834,7 +59834,7 @@
         <v>230</v>
       </c>
       <c r="M47" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
@@ -59875,7 +59875,7 @@
         <v>230</v>
       </c>
       <c r="M48" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
@@ -59916,7 +59916,7 @@
         <v>230</v>
       </c>
       <c r="M49" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -59957,7 +59957,7 @@
         <v>243</v>
       </c>
       <c r="M50" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -59998,7 +59998,7 @@
         <v>243</v>
       </c>
       <c r="M51" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -60039,7 +60039,7 @@
         <v>243</v>
       </c>
       <c r="M52" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -60080,7 +60080,7 @@
         <v>74</v>
       </c>
       <c r="M53" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -60121,7 +60121,7 @@
         <v>74</v>
       </c>
       <c r="M54" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -60162,7 +60162,7 @@
         <v>74</v>
       </c>
       <c r="M55" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -60203,7 +60203,7 @@
         <v>268</v>
       </c>
       <c r="M56" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -60244,7 +60244,7 @@
         <v>268</v>
       </c>
       <c r="M57" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -60285,7 +60285,7 @@
         <v>277</v>
       </c>
       <c r="M58" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -60326,7 +60326,7 @@
         <v>277</v>
       </c>
       <c r="M59" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
@@ -60367,7 +60367,7 @@
         <v>277</v>
       </c>
       <c r="M60" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
@@ -60408,7 +60408,7 @@
         <v>290</v>
       </c>
       <c r="M61" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
@@ -60449,7 +60449,7 @@
         <v>290</v>
       </c>
       <c r="M62" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -60490,7 +60490,7 @@
         <v>299</v>
       </c>
       <c r="M63" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
@@ -60531,7 +60531,7 @@
         <v>304</v>
       </c>
       <c r="M64" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
@@ -60572,7 +60572,7 @@
         <v>309</v>
       </c>
       <c r="M65" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
@@ -60613,7 +60613,7 @@
         <v>309</v>
       </c>
       <c r="M66" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
@@ -60654,7 +60654,7 @@
         <v>318</v>
       </c>
       <c r="M67" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
@@ -60695,7 +60695,7 @@
         <v>318</v>
       </c>
       <c r="M68" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
@@ -60736,7 +60736,7 @@
         <v>327</v>
       </c>
       <c r="M69" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
@@ -60777,7 +60777,7 @@
         <v>327</v>
       </c>
       <c r="M70" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
@@ -61474,7 +61474,7 @@
         <v>132</v>
       </c>
       <c r="M87" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
@@ -61597,7 +61597,7 @@
         <v>196</v>
       </c>
       <c r="M90" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -61638,7 +61638,7 @@
         <v>196</v>
       </c>
       <c r="M91" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
@@ -61679,7 +61679,7 @@
         <v>196</v>
       </c>
       <c r="M92" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -61720,7 +61720,7 @@
         <v>196</v>
       </c>
       <c r="M93" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
@@ -61761,7 +61761,7 @@
         <v>196</v>
       </c>
       <c r="M94" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -61802,7 +61802,7 @@
         <v>196</v>
       </c>
       <c r="M95" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -62212,7 +62212,7 @@
         <v>479</v>
       </c>
       <c r="M105" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
@@ -62253,7 +62253,7 @@
         <v>479</v>
       </c>
       <c r="M106" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -62294,7 +62294,7 @@
         <v>479</v>
       </c>
       <c r="M107" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -62335,7 +62335,7 @@
         <v>479</v>
       </c>
       <c r="M108" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
@@ -62376,7 +62376,7 @@
         <v>479</v>
       </c>
       <c r="M109" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
@@ -62417,7 +62417,7 @@
         <v>479</v>
       </c>
       <c r="M110" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -62458,7 +62458,7 @@
         <v>479</v>
       </c>
       <c r="M111" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
@@ -62499,7 +62499,7 @@
         <v>479</v>
       </c>
       <c r="M112" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
@@ -62540,7 +62540,7 @@
         <v>479</v>
       </c>
       <c r="M113" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
@@ -62581,7 +62581,7 @@
         <v>479</v>
       </c>
       <c r="M114" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
@@ -62622,7 +62622,7 @@
         <v>479</v>
       </c>
       <c r="M115" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
@@ -62663,7 +62663,7 @@
         <v>479</v>
       </c>
       <c r="M116" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
@@ -64508,7 +64508,7 @@
         <v>707</v>
       </c>
       <c r="M161" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.2">
@@ -64549,7 +64549,7 @@
         <v>712</v>
       </c>
       <c r="M162" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.2">
@@ -64590,7 +64590,7 @@
         <v>718</v>
       </c>
       <c r="M163" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.2">
@@ -64795,7 +64795,7 @@
         <v>743</v>
       </c>
       <c r="M168" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.2">
@@ -64836,7 +64836,7 @@
         <v>743</v>
       </c>
       <c r="M169" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.2">
@@ -64877,7 +64877,7 @@
         <v>743</v>
       </c>
       <c r="M170" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.2">
@@ -64918,7 +64918,7 @@
         <v>743</v>
       </c>
       <c r="M171" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.2">
@@ -64959,7 +64959,7 @@
         <v>760</v>
       </c>
       <c r="M172" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.2">
@@ -65000,7 +65000,7 @@
         <v>760</v>
       </c>
       <c r="M173" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.2">
@@ -65041,7 +65041,7 @@
         <v>760</v>
       </c>
       <c r="M174" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.2">
@@ -65082,7 +65082,7 @@
         <v>760</v>
       </c>
       <c r="M175" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.2">
@@ -65123,7 +65123,7 @@
         <v>777</v>
       </c>
       <c r="M176" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.2">
@@ -65164,7 +65164,7 @@
         <v>777</v>
       </c>
       <c r="M177" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.2">
@@ -65205,7 +65205,7 @@
         <v>777</v>
       </c>
       <c r="M178" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.2">
@@ -65328,7 +65328,7 @@
         <v>132</v>
       </c>
       <c r="M181" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.2">
@@ -65369,7 +65369,7 @@
         <v>802</v>
       </c>
       <c r="M182" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.2">
@@ -65410,7 +65410,7 @@
         <v>221</v>
       </c>
       <c r="M183" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.2">
@@ -65697,7 +65697,7 @@
         <v>838</v>
       </c>
       <c r="M190" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.2">
@@ -65820,7 +65820,7 @@
         <v>849</v>
       </c>
       <c r="M193" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.2">
@@ -65861,7 +65861,7 @@
         <v>853</v>
       </c>
       <c r="M194" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.2">
@@ -66025,7 +66025,7 @@
         <v>880</v>
       </c>
       <c r="M198" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.2">
@@ -66066,7 +66066,7 @@
         <v>884</v>
       </c>
       <c r="M199" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.2">
@@ -66189,7 +66189,7 @@
         <v>880</v>
       </c>
       <c r="M202" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.2">
@@ -66230,7 +66230,7 @@
         <v>880</v>
       </c>
       <c r="M203" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.2">
@@ -66271,7 +66271,7 @@
         <v>884</v>
       </c>
       <c r="M204" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.2">
@@ -66312,7 +66312,7 @@
         <v>884</v>
       </c>
       <c r="M205" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.2">
@@ -66394,7 +66394,7 @@
         <v>909</v>
       </c>
       <c r="M207" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.2">
@@ -66435,7 +66435,7 @@
         <v>777</v>
       </c>
       <c r="M208" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.2">
@@ -66517,7 +66517,7 @@
         <v>919</v>
       </c>
       <c r="M210" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.2">
@@ -66558,7 +66558,7 @@
         <v>923</v>
       </c>
       <c r="M211" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.2">
@@ -66599,7 +66599,7 @@
         <v>74</v>
       </c>
       <c r="M212" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.2">
@@ -66640,7 +66640,7 @@
         <v>930</v>
       </c>
       <c r="M213" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.2">
@@ -66681,7 +66681,7 @@
         <v>290</v>
       </c>
       <c r="M214" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.2">
@@ -66722,7 +66722,7 @@
         <v>937</v>
       </c>
       <c r="M215" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.2">
@@ -66763,7 +66763,7 @@
         <v>941</v>
       </c>
       <c r="M216" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.2">
@@ -66804,7 +66804,7 @@
         <v>945</v>
       </c>
       <c r="M217" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.2">
@@ -66927,7 +66927,7 @@
         <v>299</v>
       </c>
       <c r="M220" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.2">
@@ -67050,7 +67050,7 @@
         <v>965</v>
       </c>
       <c r="M223" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.2">
@@ -67911,7 +67911,7 @@
         <v>1037</v>
       </c>
       <c r="M244" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.2">
@@ -68075,7 +68075,7 @@
         <v>277</v>
       </c>
       <c r="M248" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.2">
@@ -68116,7 +68116,7 @@
         <v>1054</v>
       </c>
       <c r="M249" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.2">
@@ -68157,7 +68157,7 @@
         <v>1058</v>
       </c>
       <c r="M250" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.2">
@@ -68239,7 +68239,7 @@
         <v>1075</v>
       </c>
       <c r="M252" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.2">
@@ -68280,7 +68280,7 @@
         <v>1079</v>
       </c>
       <c r="M253" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.2">
@@ -68362,7 +68362,7 @@
         <v>1090</v>
       </c>
       <c r="M255" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.2">
@@ -68403,7 +68403,7 @@
         <v>1094</v>
       </c>
       <c r="M256" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.2">
@@ -68444,7 +68444,7 @@
         <v>1098</v>
       </c>
       <c r="M257" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.2">
@@ -68485,7 +68485,7 @@
         <v>1102</v>
       </c>
       <c r="M258" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.2">
@@ -68526,7 +68526,7 @@
         <v>1106</v>
       </c>
       <c r="M259" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.2">
@@ -68608,7 +68608,7 @@
         <v>1113</v>
       </c>
       <c r="M261" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.2">
@@ -68772,7 +68772,7 @@
         <v>1176</v>
       </c>
       <c r="M265" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="266" spans="1:13" x14ac:dyDescent="0.2">
@@ -68813,7 +68813,7 @@
         <v>1180</v>
       </c>
       <c r="M266" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.2">
@@ -68854,7 +68854,7 @@
         <v>880</v>
       </c>
       <c r="M267" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.2">
@@ -68895,7 +68895,7 @@
         <v>1187</v>
       </c>
       <c r="M268" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.2">
@@ -68936,7 +68936,7 @@
         <v>1191</v>
       </c>
       <c r="M269" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.2">
@@ -69018,7 +69018,7 @@
         <v>1198</v>
       </c>
       <c r="M271" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.2">
@@ -69059,7 +69059,7 @@
         <v>1202</v>
       </c>
       <c r="M272" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="273" spans="1:13" x14ac:dyDescent="0.2">
@@ -69100,7 +69100,7 @@
         <v>132</v>
       </c>
       <c r="M273" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.2">
@@ -70371,7 +70371,7 @@
         <v>277</v>
       </c>
       <c r="M304" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="305" spans="1:13" x14ac:dyDescent="0.2">
@@ -70412,7 +70412,7 @@
         <v>277</v>
       </c>
       <c r="M305" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.2">
@@ -70453,7 +70453,7 @@
         <v>277</v>
       </c>
       <c r="M306" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.2">
@@ -70576,7 +70576,7 @@
         <v>1464</v>
       </c>
       <c r="M309" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.2">
@@ -70617,7 +70617,7 @@
         <v>196</v>
       </c>
       <c r="M310" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.2">
@@ -70658,7 +70658,7 @@
         <v>196</v>
       </c>
       <c r="M311" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.2">
@@ -70699,7 +70699,7 @@
         <v>1474</v>
       </c>
       <c r="M312" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.2">
@@ -70740,7 +70740,7 @@
         <v>1474</v>
       </c>
       <c r="M313" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="314" spans="1:13" x14ac:dyDescent="0.2">
@@ -70781,7 +70781,7 @@
         <v>1481</v>
       </c>
       <c r="M314" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.2">
@@ -72175,7 +72175,7 @@
         <v>277</v>
       </c>
       <c r="M348" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="349" spans="1:13" x14ac:dyDescent="0.2">
@@ -72298,7 +72298,7 @@
         <v>1596</v>
       </c>
       <c r="M351" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.2">
@@ -72339,7 +72339,7 @@
         <v>1596</v>
       </c>
       <c r="M352" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="353" spans="1:13" x14ac:dyDescent="0.2">
@@ -72380,7 +72380,7 @@
         <v>1464</v>
       </c>
       <c r="M353" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="354" spans="1:13" x14ac:dyDescent="0.2">
@@ -72421,7 +72421,7 @@
         <v>196</v>
       </c>
       <c r="M354" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="355" spans="1:13" x14ac:dyDescent="0.2">
@@ -72462,7 +72462,7 @@
         <v>196</v>
       </c>
       <c r="M355" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="356" spans="1:13" x14ac:dyDescent="0.2">
@@ -72503,7 +72503,7 @@
         <v>1474</v>
       </c>
       <c r="M356" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="357" spans="1:13" x14ac:dyDescent="0.2">
@@ -72544,7 +72544,7 @@
         <v>1474</v>
       </c>
       <c r="M357" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="358" spans="1:13" x14ac:dyDescent="0.2">
@@ -72585,7 +72585,7 @@
         <v>1596</v>
       </c>
       <c r="M358" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="359" spans="1:13" x14ac:dyDescent="0.2">
@@ -72626,7 +72626,7 @@
         <v>1481</v>
       </c>
       <c r="M359" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="360" spans="1:13" x14ac:dyDescent="0.2">
@@ -72708,7 +72708,7 @@
         <v>1692</v>
       </c>
       <c r="M361" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="362" spans="1:13" x14ac:dyDescent="0.2">
@@ -72749,7 +72749,7 @@
         <v>1692</v>
       </c>
       <c r="M362" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="363" spans="1:13" x14ac:dyDescent="0.2">
@@ -72790,7 +72790,7 @@
         <v>1692</v>
       </c>
       <c r="M363" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="364" spans="1:13" x14ac:dyDescent="0.2">
@@ -72831,7 +72831,7 @@
         <v>1692</v>
       </c>
       <c r="M364" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="365" spans="1:13" x14ac:dyDescent="0.2">
@@ -72954,7 +72954,7 @@
         <v>1474</v>
       </c>
       <c r="M367" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="368" spans="1:13" x14ac:dyDescent="0.2">
@@ -72995,7 +72995,7 @@
         <v>1474</v>
       </c>
       <c r="M368" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="369" spans="1:13" x14ac:dyDescent="0.2">
@@ -73036,7 +73036,7 @@
         <v>1474</v>
       </c>
       <c r="M369" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="370" spans="1:13" x14ac:dyDescent="0.2">
@@ -73077,7 +73077,7 @@
         <v>1474</v>
       </c>
       <c r="M370" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="371" spans="1:13" x14ac:dyDescent="0.2">
@@ -73118,7 +73118,7 @@
         <v>1724</v>
       </c>
       <c r="M371" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.2">
@@ -73159,7 +73159,7 @@
         <v>1724</v>
       </c>
       <c r="M372" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="373" spans="1:13" x14ac:dyDescent="0.2">
@@ -73241,7 +73241,7 @@
         <v>1596</v>
       </c>
       <c r="M374" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.2">
@@ -73282,7 +73282,7 @@
         <v>1464</v>
       </c>
       <c r="M375" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="376" spans="1:13" x14ac:dyDescent="0.2">
@@ -73323,7 +73323,7 @@
         <v>1741</v>
       </c>
       <c r="M376" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="377" spans="1:13" x14ac:dyDescent="0.2">
@@ -73364,7 +73364,7 @@
         <v>1741</v>
       </c>
       <c r="M377" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="378" spans="1:13" x14ac:dyDescent="0.2">
@@ -73405,7 +73405,7 @@
         <v>230</v>
       </c>
       <c r="M378" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="379" spans="1:13" x14ac:dyDescent="0.2">
@@ -73446,7 +73446,7 @@
         <v>479</v>
       </c>
       <c r="M379" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="380" spans="1:13" x14ac:dyDescent="0.2">
@@ -73487,7 +73487,7 @@
         <v>479</v>
       </c>
       <c r="M380" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="381" spans="1:13" x14ac:dyDescent="0.2">
@@ -73528,7 +73528,7 @@
         <v>1757</v>
       </c>
       <c r="M381" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="382" spans="1:13" x14ac:dyDescent="0.2">
@@ -73569,7 +73569,7 @@
         <v>1761</v>
       </c>
       <c r="M382" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="383" spans="1:13" x14ac:dyDescent="0.2">
@@ -73610,7 +73610,7 @@
         <v>1765</v>
       </c>
       <c r="M383" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="384" spans="1:13" x14ac:dyDescent="0.2">
@@ -73692,7 +73692,7 @@
         <v>1773</v>
       </c>
       <c r="M385" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="386" spans="1:13" x14ac:dyDescent="0.2">
@@ -73815,7 +73815,7 @@
         <v>1785</v>
       </c>
       <c r="M388" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="389" spans="1:13" x14ac:dyDescent="0.2">
@@ -73856,7 +73856,7 @@
         <v>1793</v>
       </c>
       <c r="M389" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.2">
@@ -73938,7 +73938,7 @@
         <v>1801</v>
       </c>
       <c r="M391" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.2">
@@ -73979,7 +73979,7 @@
         <v>1805</v>
       </c>
       <c r="M392" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="393" spans="1:13" x14ac:dyDescent="0.2">
@@ -74061,7 +74061,7 @@
         <v>1481</v>
       </c>
       <c r="M394" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="395" spans="1:13" x14ac:dyDescent="0.2">
@@ -74143,7 +74143,7 @@
         <v>1819</v>
       </c>
       <c r="M396" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="397" spans="1:13" x14ac:dyDescent="0.2">
@@ -74225,7 +74225,7 @@
         <v>1481</v>
       </c>
       <c r="M398" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="399" spans="1:13" x14ac:dyDescent="0.2">
@@ -74307,7 +74307,7 @@
         <v>945</v>
       </c>
       <c r="M400" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="401" spans="1:13" x14ac:dyDescent="0.2">
@@ -74471,7 +74471,7 @@
         <v>1847</v>
       </c>
       <c r="M404" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="405" spans="1:13" x14ac:dyDescent="0.2">
@@ -74512,7 +74512,7 @@
         <v>268</v>
       </c>
       <c r="M405" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="406" spans="1:13" x14ac:dyDescent="0.2">
@@ -74553,7 +74553,7 @@
         <v>1692</v>
       </c>
       <c r="M406" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="407" spans="1:13" x14ac:dyDescent="0.2">
@@ -74635,7 +74635,7 @@
         <v>884</v>
       </c>
       <c r="M408" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="409" spans="1:13" x14ac:dyDescent="0.2">
@@ -74717,7 +74717,7 @@
         <v>884</v>
       </c>
       <c r="M410" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="411" spans="1:13" x14ac:dyDescent="0.2">
@@ -77874,7 +77874,7 @@
         <v>880</v>
       </c>
       <c r="M487" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="488" spans="1:13" x14ac:dyDescent="0.2">
@@ -77915,7 +77915,7 @@
         <v>884</v>
       </c>
       <c r="M488" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="489" spans="1:13" x14ac:dyDescent="0.2">
@@ -78284,7 +78284,7 @@
         <v>2158</v>
       </c>
       <c r="M497" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N497" t="s">
         <v>2159</v>
@@ -78328,7 +78328,7 @@
         <v>277</v>
       </c>
       <c r="M498" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N498" t="s">
         <v>2164</v>
@@ -78413,7 +78413,7 @@
         <v>2174</v>
       </c>
       <c r="M500" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N500" t="s">
         <v>2175</v>
@@ -78498,7 +78498,7 @@
         <v>1847</v>
       </c>
       <c r="M502" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N502" t="s">
         <v>2184</v>
@@ -78542,7 +78542,7 @@
         <v>74</v>
       </c>
       <c r="M503" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N503" t="s">
         <v>2189</v>
@@ -78586,7 +78586,7 @@
         <v>1102</v>
       </c>
       <c r="M504" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="505" spans="1:14" x14ac:dyDescent="0.2">
@@ -78627,7 +78627,7 @@
         <v>2198</v>
       </c>
       <c r="M505" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="506" spans="1:14" x14ac:dyDescent="0.2">
@@ -78668,7 +78668,7 @@
         <v>2203</v>
       </c>
       <c r="M506" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N506" t="s">
         <v>2204</v>
@@ -78712,7 +78712,7 @@
         <v>1481</v>
       </c>
       <c r="M507" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N507" t="s">
         <v>2209</v>
@@ -78797,7 +78797,7 @@
         <v>2217</v>
       </c>
       <c r="M509" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N509" t="s">
         <v>2218</v>
@@ -78882,7 +78882,7 @@
         <v>196</v>
       </c>
       <c r="M511" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="512" spans="1:14" x14ac:dyDescent="0.2">
@@ -78923,7 +78923,7 @@
         <v>2231</v>
       </c>
       <c r="M512" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
       <c r="N512" t="s">
         <v>2233</v>
@@ -78967,7 +78967,7 @@
         <v>299</v>
       </c>
       <c r="M513" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="514" spans="1:14" x14ac:dyDescent="0.2">
@@ -79008,7 +79008,7 @@
         <v>1079</v>
       </c>
       <c r="M514" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="515" spans="1:14" x14ac:dyDescent="0.2">
@@ -79049,7 +79049,7 @@
         <v>1757</v>
       </c>
       <c r="M515" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="516" spans="1:14" x14ac:dyDescent="0.2">
@@ -79090,7 +79090,7 @@
         <v>2250</v>
       </c>
       <c r="M516" t="s">
-        <v>75</v>
+        <v>2302</v>
       </c>
       <c r="N516" t="s">
         <v>2251</v>
@@ -79380,7 +79380,7 @@
         <v>2294</v>
       </c>
       <c r="M523" t="s">
-        <v>133</v>
+        <v>2301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates before swutching to main branch
</commit_message>
<xml_diff>
--- a/cichlid_sr_sequencing/SampleDatabase.xlsx
+++ b/cichlid_sr_sequencing/SampleDatabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmnike/Desktop/VCF_Excel_Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmnike/CichlidSRSequencing/cichlid_sr_sequencing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7502FE0-3E3C-0C4D-9BCC-65DBDC68C726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EFFB3D-5A8B-9D44-BCB9-E87D67B3BC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33580" yWindow="540" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="540" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDatabase_Fixed_Ecogroups" sheetId="1" r:id="rId1"/>
@@ -7143,11 +7143,11 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60805,8 +60805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D116E73-55E3-504B-8741-15E6858173B5}">
   <dimension ref="A1:U523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -61011,7 +61011,7 @@
       <c r="P3" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q3" s="27">
+      <c r="Q3" s="29">
         <v>9</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -61076,7 +61076,7 @@
       <c r="P4" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q4" s="27"/>
+      <c r="Q4" s="29"/>
       <c r="R4" s="3" t="s">
         <v>251</v>
       </c>
@@ -61139,7 +61139,7 @@
       <c r="P5" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q5" s="27"/>
+      <c r="Q5" s="29"/>
       <c r="R5" s="3" t="s">
         <v>492</v>
       </c>
@@ -61202,7 +61202,7 @@
       <c r="P6" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="29"/>
       <c r="R6" s="3" t="s">
         <v>2285</v>
       </c>
@@ -61265,7 +61265,7 @@
       <c r="P7" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q7" s="27"/>
+      <c r="Q7" s="29"/>
       <c r="R7" s="3" t="s">
         <v>2286</v>
       </c>
@@ -61328,7 +61328,7 @@
       <c r="P8" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q8" s="27"/>
+      <c r="Q8" s="29"/>
       <c r="R8" s="3" t="s">
         <v>218</v>
       </c>
@@ -61391,7 +61391,7 @@
       <c r="P9" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q9" s="27"/>
+      <c r="Q9" s="29"/>
       <c r="R9" s="3" t="s">
         <v>181</v>
       </c>
@@ -61454,7 +61454,7 @@
       <c r="P10" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q10" s="27"/>
+      <c r="Q10" s="29"/>
       <c r="R10" s="3" t="s">
         <v>2293</v>
       </c>
@@ -61512,7 +61512,7 @@
       <c r="P11" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="Q11" s="27"/>
+      <c r="Q11" s="29"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -72771,46 +72771,46 @@
       </c>
     </row>
     <row r="266" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A266" s="29" t="s">
+      <c r="A266" s="28" t="s">
         <v>1213</v>
       </c>
-      <c r="B266" s="29" t="s">
+      <c r="B266" s="28" t="s">
         <v>1214</v>
       </c>
-      <c r="C266" s="29">
+      <c r="C266" s="28">
         <v>250</v>
       </c>
-      <c r="D266" s="29">
+      <c r="D266" s="28">
         <v>16219305500</v>
       </c>
-      <c r="E266" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F266" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G266" s="29">
+      <c r="E266" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F266" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G266" s="28">
         <v>11649550</v>
       </c>
-      <c r="H266" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I266" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="J266" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K266" s="29" t="s">
+      <c r="H266" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I266" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="J266" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K266" s="28" t="s">
         <v>1215</v>
       </c>
-      <c r="L266" s="29" t="s">
+      <c r="L266" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="M266" s="29" t="s">
+      <c r="M266" s="28" t="s">
         <v>2285</v>
       </c>
-      <c r="N266" s="29" t="s">
+      <c r="N266" s="28" t="s">
         <v>2300</v>
       </c>
     </row>
@@ -78184,46 +78184,46 @@
       </c>
     </row>
     <row r="389" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A389" s="28" t="s">
+      <c r="A389" s="27" t="s">
         <v>1751</v>
       </c>
-      <c r="B389" s="28" t="s">
+      <c r="B389" s="27" t="s">
         <v>1752</v>
       </c>
-      <c r="C389" s="28">
+      <c r="C389" s="27">
         <v>250</v>
       </c>
-      <c r="D389" s="28">
+      <c r="D389" s="27">
         <v>16219846000</v>
       </c>
-      <c r="E389" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F389" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G389" s="28">
+      <c r="E389" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F389" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G389" s="27">
         <v>11649599</v>
       </c>
-      <c r="H389" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="I389" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="J389" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="K389" s="28" t="s">
+      <c r="H389" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I389" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J389" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K389" s="27" t="s">
         <v>1753</v>
       </c>
-      <c r="L389" s="28" t="s">
+      <c r="L389" s="27" t="s">
         <v>387</v>
       </c>
-      <c r="M389" s="28" t="s">
+      <c r="M389" s="27" t="s">
         <v>2285</v>
       </c>
-      <c r="N389" s="28" t="s">
+      <c r="N389" s="27" t="s">
         <v>2300</v>
       </c>
     </row>
@@ -80340,46 +80340,46 @@
       </c>
     </row>
     <row r="438" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A438" s="28" t="s">
+      <c r="A438" s="27" t="s">
         <v>1953</v>
       </c>
-      <c r="B438" s="28" t="s">
+      <c r="B438" s="27" t="s">
         <v>1954</v>
       </c>
-      <c r="C438" s="28">
+      <c r="C438" s="27">
         <v>200</v>
       </c>
-      <c r="D438" s="28">
+      <c r="D438" s="27">
         <v>5025224400</v>
       </c>
-      <c r="E438" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F438" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G438" s="28">
+      <c r="E438" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F438" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G438" s="27">
         <v>6526445</v>
       </c>
-      <c r="H438" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="I438" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="J438" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="K438" s="28" t="s">
+      <c r="H438" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I438" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J438" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K438" s="27" t="s">
         <v>1955</v>
       </c>
-      <c r="L438" s="28" t="s">
+      <c r="L438" s="27" t="s">
         <v>471</v>
       </c>
-      <c r="M438" s="28" t="s">
+      <c r="M438" s="27" t="s">
         <v>2286</v>
       </c>
-      <c r="N438" s="28" t="s">
+      <c r="N438" s="27" t="s">
         <v>2300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
uncommented lines in alignFastq.py
</commit_message>
<xml_diff>
--- a/cichlid_sr_sequencing/SampleDatabase.xlsx
+++ b/cichlid_sr_sequencing/SampleDatabase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10305"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmnike/CichlidSRSequencing/cichlid_sr_sequencing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EFFB3D-5A8B-9D44-BCB9-E87D67B3BC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C6177D-7E20-8447-A576-F83F290301FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="540" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDatabase_Fixed_Ecogroups" sheetId="1" r:id="rId1"/>
@@ -37674,8 +37674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F40BAC0-9C48-CA42-B6D8-635F339212A2}">
   <dimension ref="A1:N525"/>
   <sheetViews>
-    <sheetView topLeftCell="A414" workbookViewId="0">
-      <selection activeCell="L440" sqref="L440"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -60803,10 +60803,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D116E73-55E3-504B-8741-15E6858173B5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView topLeftCell="D1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="M201" sqref="M201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -60897,7 +60898,7 @@
         <v>2296</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -60962,7 +60963,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -61027,7 +61028,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
@@ -61090,7 +61091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -61153,7 +61154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
@@ -61216,7 +61217,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>56</v>
       </c>
@@ -61279,7 +61280,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -61342,7 +61343,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>64</v>
       </c>
@@ -61405,7 +61406,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>68</v>
       </c>
@@ -61463,7 +61464,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>73</v>
       </c>
@@ -61514,7 +61515,7 @@
       </c>
       <c r="Q11" s="29"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>77</v>
       </c>
@@ -61567,7 +61568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>81</v>
       </c>
@@ -61620,7 +61621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>85</v>
       </c>
@@ -61673,7 +61674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>89</v>
       </c>
@@ -61726,7 +61727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>93</v>
       </c>
@@ -61779,7 +61780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>97</v>
       </c>
@@ -61832,7 +61833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
@@ -61885,7 +61886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>105</v>
       </c>
@@ -61938,7 +61939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>109</v>
       </c>
@@ -61990,7 +61991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>113</v>
       </c>
@@ -62034,7 +62035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>117</v>
       </c>
@@ -62078,7 +62079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>121</v>
       </c>
@@ -62122,7 +62123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>125</v>
       </c>
@@ -62166,7 +62167,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>129</v>
       </c>
@@ -62210,7 +62211,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>133</v>
       </c>
@@ -62254,7 +62255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>137</v>
       </c>
@@ -62298,7 +62299,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>141</v>
       </c>
@@ -62342,7 +62343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>145</v>
       </c>
@@ -62386,7 +62387,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>149</v>
       </c>
@@ -62430,7 +62431,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>153</v>
       </c>
@@ -62474,7 +62475,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>157</v>
       </c>
@@ -62518,7 +62519,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>161</v>
       </c>
@@ -62562,7 +62563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>165</v>
       </c>
@@ -62606,7 +62607,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>169</v>
       </c>
@@ -62650,7 +62651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>173</v>
       </c>
@@ -62694,7 +62695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>177</v>
       </c>
@@ -62738,7 +62739,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>182</v>
       </c>
@@ -62782,7 +62783,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>186</v>
       </c>
@@ -62826,7 +62827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>190</v>
       </c>
@@ -62870,7 +62871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>194</v>
       </c>
@@ -62914,7 +62915,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>198</v>
       </c>
@@ -62958,7 +62959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>202</v>
       </c>
@@ -63002,7 +63003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>206</v>
       </c>
@@ -63046,7 +63047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>210</v>
       </c>
@@ -63090,7 +63091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>214</v>
       </c>
@@ -63134,7 +63135,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>219</v>
       </c>
@@ -63178,7 +63179,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>223</v>
       </c>
@@ -63222,7 +63223,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>227</v>
       </c>
@@ -63266,7 +63267,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>231</v>
       </c>
@@ -63310,7 +63311,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>235</v>
       </c>
@@ -63354,7 +63355,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>239</v>
       </c>
@@ -63398,7 +63399,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>243</v>
       </c>
@@ -63442,7 +63443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>247</v>
       </c>
@@ -63486,7 +63487,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>252</v>
       </c>
@@ -63530,7 +63531,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>256</v>
       </c>
@@ -63574,7 +63575,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>260</v>
       </c>
@@ -63618,7 +63619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>264</v>
       </c>
@@ -63662,7 +63663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>268</v>
       </c>
@@ -63706,7 +63707,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>272</v>
       </c>
@@ -63750,7 +63751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>276</v>
       </c>
@@ -63794,7 +63795,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>280</v>
       </c>
@@ -63838,7 +63839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>284</v>
       </c>
@@ -63882,7 +63883,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>288</v>
       </c>
@@ -63926,7 +63927,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>292</v>
       </c>
@@ -63970,7 +63971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>296</v>
       </c>
@@ -64014,7 +64015,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>300</v>
       </c>
@@ -64058,7 +64059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>304</v>
       </c>
@@ -64102,7 +64103,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>308</v>
       </c>
@@ -64146,7 +64147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>312</v>
       </c>
@@ -64190,7 +64191,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>316</v>
       </c>
@@ -64234,7 +64235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>320</v>
       </c>
@@ -64278,7 +64279,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>324</v>
       </c>
@@ -64322,7 +64323,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>328</v>
       </c>
@@ -64366,7 +64367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>332</v>
       </c>
@@ -64410,7 +64411,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>336</v>
       </c>
@@ -64454,7 +64455,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>340</v>
       </c>
@@ -64498,7 +64499,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>344</v>
       </c>
@@ -64542,7 +64543,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>348</v>
       </c>
@@ -64586,7 +64587,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>352</v>
       </c>
@@ -64630,7 +64631,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>356</v>
       </c>
@@ -64674,7 +64675,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>360</v>
       </c>
@@ -64718,7 +64719,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>364</v>
       </c>
@@ -64762,7 +64763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>368</v>
       </c>
@@ -64806,7 +64807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>372</v>
       </c>
@@ -64850,7 +64851,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>376</v>
       </c>
@@ -64894,7 +64895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>380</v>
       </c>
@@ -64938,7 +64939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>384</v>
       </c>
@@ -64982,7 +64983,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>388</v>
       </c>
@@ -65026,7 +65027,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>392</v>
       </c>
@@ -65070,7 +65071,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>396</v>
       </c>
@@ -65114,7 +65115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>400</v>
       </c>
@@ -65158,7 +65159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>404</v>
       </c>
@@ -65202,7 +65203,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>408</v>
       </c>
@@ -65246,7 +65247,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>412</v>
       </c>
@@ -65290,7 +65291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>416</v>
       </c>
@@ -65334,7 +65335,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>420</v>
       </c>
@@ -65378,7 +65379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>424</v>
       </c>
@@ -65422,7 +65423,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>428</v>
       </c>
@@ -65466,7 +65467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>432</v>
       </c>
@@ -65510,7 +65511,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>436</v>
       </c>
@@ -65554,7 +65555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>440</v>
       </c>
@@ -65598,7 +65599,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>444</v>
       </c>
@@ -65642,7 +65643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>448</v>
       </c>
@@ -65686,7 +65687,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>452</v>
       </c>
@@ -65730,7 +65731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>456</v>
       </c>
@@ -65774,7 +65775,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>460</v>
       </c>
@@ -65818,7 +65819,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>464</v>
       </c>
@@ -65862,7 +65863,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>468</v>
       </c>
@@ -65906,7 +65907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>472</v>
       </c>
@@ -65950,7 +65951,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>476</v>
       </c>
@@ -65994,7 +65995,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>480</v>
       </c>
@@ -66038,7 +66039,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>484</v>
       </c>
@@ -66082,7 +66083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>488</v>
       </c>
@@ -66126,7 +66127,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>493</v>
       </c>
@@ -66170,7 +66171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>497</v>
       </c>
@@ -66214,7 +66215,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>501</v>
       </c>
@@ -66258,7 +66259,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>505</v>
       </c>
@@ -66302,7 +66303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>509</v>
       </c>
@@ -66346,7 +66347,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>513</v>
       </c>
@@ -66390,7 +66391,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>517</v>
       </c>
@@ -66434,7 +66435,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>521</v>
       </c>
@@ -66478,7 +66479,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>525</v>
       </c>
@@ -66522,7 +66523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>529</v>
       </c>
@@ -66566,7 +66567,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>533</v>
       </c>
@@ -66610,7 +66611,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>537</v>
       </c>
@@ -66654,7 +66655,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>541</v>
       </c>
@@ -66698,7 +66699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>545</v>
       </c>
@@ -66742,7 +66743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>549</v>
       </c>
@@ -66786,7 +66787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>553</v>
       </c>
@@ -66830,7 +66831,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>557</v>
       </c>
@@ -66874,7 +66875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>561</v>
       </c>
@@ -66918,7 +66919,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>565</v>
       </c>
@@ -66962,7 +66963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>569</v>
       </c>
@@ -67006,7 +67007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>572</v>
       </c>
@@ -67050,7 +67051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>575</v>
       </c>
@@ -67094,7 +67095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>578</v>
       </c>
@@ -67138,7 +67139,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>581</v>
       </c>
@@ -67182,7 +67183,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>584</v>
       </c>
@@ -67226,7 +67227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>590</v>
       </c>
@@ -67270,7 +67271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>593</v>
       </c>
@@ -67314,7 +67315,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>596</v>
       </c>
@@ -67358,7 +67359,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>599</v>
       </c>
@@ -67402,7 +67403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>602</v>
       </c>
@@ -67446,7 +67447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>606</v>
       </c>
@@ -67490,7 +67491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>610</v>
       </c>
@@ -67534,7 +67535,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>614</v>
       </c>
@@ -67578,7 +67579,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>617</v>
       </c>
@@ -67622,7 +67623,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>620</v>
       </c>
@@ -67666,7 +67667,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>625</v>
       </c>
@@ -67710,7 +67711,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>630</v>
       </c>
@@ -67754,7 +67755,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>633</v>
       </c>
@@ -67798,7 +67799,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>636</v>
       </c>
@@ -67842,7 +67843,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>691</v>
       </c>
@@ -67886,7 +67887,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>694</v>
       </c>
@@ -67930,7 +67931,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>697</v>
       </c>
@@ -67974,7 +67975,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>700</v>
       </c>
@@ -68018,7 +68019,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>703</v>
       </c>
@@ -68062,7 +68063,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>706</v>
       </c>
@@ -68106,7 +68107,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>709</v>
       </c>
@@ -68150,7 +68151,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>712</v>
       </c>
@@ -68194,7 +68195,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>715</v>
       </c>
@@ -68238,7 +68239,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>718</v>
       </c>
@@ -68282,7 +68283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>721</v>
       </c>
@@ -68326,7 +68327,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>724</v>
       </c>
@@ -68370,7 +68371,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>727</v>
       </c>
@@ -68414,7 +68415,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>730</v>
       </c>
@@ -68458,7 +68459,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>733</v>
       </c>
@@ -68502,7 +68503,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>744</v>
       </c>
@@ -68546,7 +68547,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>749</v>
       </c>
@@ -68590,7 +68591,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>752</v>
       </c>
@@ -68634,7 +68635,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>755</v>
       </c>
@@ -68678,7 +68679,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>758</v>
       </c>
@@ -68722,7 +68723,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>761</v>
       </c>
@@ -68766,7 +68767,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>764</v>
       </c>
@@ -68810,7 +68811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>767</v>
       </c>
@@ -68854,7 +68855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>770</v>
       </c>
@@ -68898,7 +68899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>777</v>
       </c>
@@ -68942,7 +68943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>780</v>
       </c>
@@ -68986,7 +68987,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>803</v>
       </c>
@@ -69030,7 +69031,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>806</v>
       </c>
@@ -69074,7 +69075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>813</v>
       </c>
@@ -69118,7 +69119,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>816</v>
       </c>
@@ -69162,7 +69163,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>819</v>
       </c>
@@ -69206,7 +69207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>834</v>
       </c>
@@ -69250,7 +69251,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>845</v>
       </c>
@@ -69294,7 +69295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>849</v>
       </c>
@@ -69338,7 +69339,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>853</v>
       </c>
@@ -69382,7 +69383,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>857</v>
       </c>
@@ -69426,7 +69427,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>861</v>
       </c>
@@ -69470,7 +69471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>865</v>
       </c>
@@ -69514,7 +69515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>868</v>
       </c>
@@ -69558,7 +69559,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>872</v>
       </c>
@@ -69602,7 +69603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>876</v>
       </c>
@@ -69646,7 +69647,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>880</v>
       </c>
@@ -69690,7 +69691,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>884</v>
       </c>
@@ -69734,7 +69735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>888</v>
       </c>
@@ -69778,7 +69779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>892</v>
       </c>
@@ -69822,7 +69823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>896</v>
       </c>
@@ -70438,7 +70439,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>1003</v>
       </c>
@@ -70482,7 +70483,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>1007</v>
       </c>
@@ -70526,7 +70527,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>1011</v>
       </c>
@@ -70570,7 +70571,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>1015</v>
       </c>
@@ -70614,7 +70615,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>1018</v>
       </c>
@@ -70658,7 +70659,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>1025</v>
       </c>
@@ -70702,7 +70703,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>1028</v>
       </c>
@@ -70746,7 +70747,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>1031</v>
       </c>
@@ -70790,7 +70791,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>1036</v>
       </c>
@@ -70834,7 +70835,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>1039</v>
       </c>
@@ -70878,7 +70879,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>1042</v>
       </c>
@@ -70922,7 +70923,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>1045</v>
       </c>
@@ -70966,7 +70967,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>1048</v>
       </c>
@@ -71010,7 +71011,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>1051</v>
       </c>
@@ -71054,7 +71055,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>1055</v>
       </c>
@@ -71098,7 +71099,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="26" t="s">
         <v>1059</v>
       </c>
@@ -71142,7 +71143,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="26" t="s">
         <v>1066</v>
       </c>
@@ -71186,7 +71187,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>1070</v>
       </c>
@@ -71230,7 +71231,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>1077</v>
       </c>
@@ -71274,7 +71275,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>1080</v>
       </c>
@@ -71318,7 +71319,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>1084</v>
       </c>
@@ -71362,7 +71363,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>1088</v>
       </c>
@@ -71406,7 +71407,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>1092</v>
       </c>
@@ -71450,7 +71451,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>1096</v>
       </c>
@@ -71494,7 +71495,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
         <v>1100</v>
       </c>
@@ -71538,7 +71539,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
         <v>1104</v>
       </c>
@@ -71582,7 +71583,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
         <v>1108</v>
       </c>
@@ -71626,7 +71627,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
         <v>1112</v>
       </c>
@@ -71670,7 +71671,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
         <v>1116</v>
       </c>
@@ -71714,7 +71715,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>1120</v>
       </c>
@@ -71758,7 +71759,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>1124</v>
       </c>
@@ -71802,7 +71803,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>1128</v>
       </c>
@@ -71846,7 +71847,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>1132</v>
       </c>
@@ -71890,7 +71891,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>1136</v>
       </c>
@@ -71934,7 +71935,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>1140</v>
       </c>
@@ -71978,7 +71979,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>1144</v>
       </c>
@@ -72022,7 +72023,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>1148</v>
       </c>
@@ -72066,7 +72067,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>1152</v>
       </c>
@@ -72110,7 +72111,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>1157</v>
       </c>
@@ -72154,7 +72155,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>1160</v>
       </c>
@@ -72198,7 +72199,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>1163</v>
       </c>
@@ -72242,7 +72243,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>1166</v>
       </c>
@@ -72286,7 +72287,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>1171</v>
       </c>
@@ -72330,7 +72331,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>1175</v>
       </c>
@@ -72374,7 +72375,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>1181</v>
       </c>
@@ -72418,7 +72419,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>1187</v>
       </c>
@@ -72462,7 +72463,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>1190</v>
       </c>
@@ -72506,7 +72507,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>1193</v>
       </c>
@@ -72550,7 +72551,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>1197</v>
       </c>
@@ -72594,7 +72595,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>1200</v>
       </c>
@@ -72638,7 +72639,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>1203</v>
       </c>
@@ -72682,7 +72683,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>1206</v>
       </c>
@@ -72726,7 +72727,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>1209</v>
       </c>
@@ -72770,7 +72771,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="28" t="s">
         <v>1213</v>
       </c>
@@ -72814,7 +72815,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>1216</v>
       </c>
@@ -72858,7 +72859,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>1220</v>
       </c>
@@ -72902,7 +72903,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>1223</v>
       </c>
@@ -72946,7 +72947,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>1227</v>
       </c>
@@ -72990,7 +72991,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>1230</v>
       </c>
@@ -73034,7 +73035,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
         <v>1234</v>
       </c>
@@ -73078,7 +73079,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>1238</v>
       </c>
@@ -73122,7 +73123,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
         <v>1241</v>
       </c>
@@ -73166,7 +73167,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>1245</v>
       </c>
@@ -73210,7 +73211,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
         <v>1249</v>
       </c>
@@ -73254,7 +73255,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>1253</v>
       </c>
@@ -73298,7 +73299,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
         <v>1257</v>
       </c>
@@ -73342,7 +73343,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>1261</v>
       </c>
@@ -73386,7 +73387,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
         <v>1264</v>
       </c>
@@ -73430,7 +73431,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>1268</v>
       </c>
@@ -73474,7 +73475,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
         <v>1272</v>
       </c>
@@ -73518,7 +73519,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="4" t="s">
         <v>1276</v>
       </c>
@@ -73562,7 +73563,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
         <v>1279</v>
       </c>
@@ -73607,7 +73608,7 @@
       </c>
       <c r="O284" s="5"/>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>1282</v>
       </c>
@@ -73651,7 +73652,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
         <v>1286</v>
       </c>
@@ -73695,7 +73696,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
         <v>1290</v>
       </c>
@@ -73739,7 +73740,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
         <v>1294</v>
       </c>
@@ -73783,7 +73784,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
         <v>1298</v>
       </c>
@@ -73827,7 +73828,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
         <v>1302</v>
       </c>
@@ -73871,7 +73872,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
         <v>1306</v>
       </c>
@@ -73915,7 +73916,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
         <v>1310</v>
       </c>
@@ -73959,7 +73960,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>1314</v>
       </c>
@@ -74003,7 +74004,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
         <v>1318</v>
       </c>
@@ -74047,7 +74048,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>1322</v>
       </c>
@@ -74091,7 +74092,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
         <v>1326</v>
       </c>
@@ -74135,7 +74136,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
         <v>1330</v>
       </c>
@@ -74179,7 +74180,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
         <v>1334</v>
       </c>
@@ -74223,7 +74224,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
         <v>1338</v>
       </c>
@@ -74267,7 +74268,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
         <v>1342</v>
       </c>
@@ -74311,7 +74312,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
         <v>1346</v>
       </c>
@@ -74355,7 +74356,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
         <v>1349</v>
       </c>
@@ -74399,7 +74400,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
         <v>1353</v>
       </c>
@@ -74443,7 +74444,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
         <v>1356</v>
       </c>
@@ -74487,7 +74488,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
         <v>1359</v>
       </c>
@@ -74531,7 +74532,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
         <v>1363</v>
       </c>
@@ -74575,7 +74576,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
         <v>1367</v>
       </c>
@@ -74619,7 +74620,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
         <v>1371</v>
       </c>
@@ -74663,7 +74664,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="309" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
         <v>1375</v>
       </c>
@@ -74707,7 +74708,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
         <v>1379</v>
       </c>
@@ -74751,7 +74752,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
         <v>1382</v>
       </c>
@@ -74795,7 +74796,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" s="3" t="s">
         <v>1385</v>
       </c>
@@ -74839,7 +74840,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
         <v>1388</v>
       </c>
@@ -74883,7 +74884,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" s="3" t="s">
         <v>1391</v>
       </c>
@@ -74927,7 +74928,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
         <v>1395</v>
       </c>
@@ -74971,7 +74972,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" s="3" t="s">
         <v>1398</v>
       </c>
@@ -75015,7 +75016,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="317" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" s="4" t="s">
         <v>1402</v>
       </c>
@@ -75059,7 +75060,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" s="3" t="s">
         <v>1406</v>
       </c>
@@ -75103,7 +75104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
         <v>1410</v>
       </c>
@@ -75147,7 +75148,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" s="3" t="s">
         <v>1413</v>
       </c>
@@ -75191,7 +75192,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
         <v>1416</v>
       </c>
@@ -75235,7 +75236,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" s="3" t="s">
         <v>1419</v>
       </c>
@@ -75279,7 +75280,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
         <v>1422</v>
       </c>
@@ -75323,7 +75324,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" s="4" t="s">
         <v>1425</v>
       </c>
@@ -75367,7 +75368,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" s="4" t="s">
         <v>1429</v>
       </c>
@@ -75411,7 +75412,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" s="4" t="s">
         <v>1433</v>
       </c>
@@ -75455,7 +75456,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" s="4" t="s">
         <v>1437</v>
       </c>
@@ -75499,7 +75500,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
         <v>1441</v>
       </c>
@@ -75543,7 +75544,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" s="4" t="s">
         <v>1445</v>
       </c>
@@ -75587,7 +75588,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="330" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" s="4" t="s">
         <v>1449</v>
       </c>
@@ -75631,7 +75632,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" s="4" t="s">
         <v>1453</v>
       </c>
@@ -75675,7 +75676,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="332" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" s="4" t="s">
         <v>1457</v>
       </c>
@@ -75719,7 +75720,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
         <v>1461</v>
       </c>
@@ -75763,7 +75764,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="s">
         <v>1465</v>
       </c>
@@ -75807,7 +75808,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
         <v>1468</v>
       </c>
@@ -75851,7 +75852,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="s">
         <v>1475</v>
       </c>
@@ -75895,7 +75896,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
         <v>1482</v>
       </c>
@@ -75939,7 +75940,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="338" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" s="3" t="s">
         <v>1486</v>
       </c>
@@ -75983,7 +75984,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
         <v>1490</v>
       </c>
@@ -76027,7 +76028,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" s="3" t="s">
         <v>1494</v>
       </c>
@@ -76071,7 +76072,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>1501</v>
       </c>
@@ -76115,7 +76116,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" s="3" t="s">
         <v>1504</v>
       </c>
@@ -76159,7 +76160,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
         <v>1507</v>
       </c>
@@ -76203,7 +76204,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="344" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" s="3" t="s">
         <v>1510</v>
       </c>
@@ -76247,7 +76248,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="345" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
         <v>1565</v>
       </c>
@@ -76291,7 +76292,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="346" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" s="3" t="s">
         <v>1568</v>
       </c>
@@ -76335,7 +76336,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="347" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
         <v>1575</v>
       </c>
@@ -76379,7 +76380,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="348" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" s="3" t="s">
         <v>1579</v>
       </c>
@@ -76423,7 +76424,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="349" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
         <v>1583</v>
       </c>
@@ -76467,7 +76468,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="350" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" s="3" t="s">
         <v>1590</v>
       </c>
@@ -76511,7 +76512,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="351" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
         <v>1594</v>
       </c>
@@ -76555,7 +76556,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="352" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" s="3" t="s">
         <v>1598</v>
       </c>
@@ -76599,7 +76600,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="353" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
         <v>1602</v>
       </c>
@@ -76643,7 +76644,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="354" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" s="3" t="s">
         <v>1606</v>
       </c>
@@ -76687,7 +76688,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="355" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
         <v>1610</v>
       </c>
@@ -76731,7 +76732,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="356" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" s="3" t="s">
         <v>1614</v>
       </c>
@@ -76775,7 +76776,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="357" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
         <v>1618</v>
       </c>
@@ -76819,7 +76820,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="358" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" s="3" t="s">
         <v>1622</v>
       </c>
@@ -76863,7 +76864,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="359" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
         <v>1626</v>
       </c>
@@ -76907,7 +76908,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="360" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" s="3" t="s">
         <v>1630</v>
       </c>
@@ -76951,7 +76952,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="361" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
         <v>1634</v>
       </c>
@@ -76995,7 +76996,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="362" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" s="3" t="s">
         <v>1638</v>
       </c>
@@ -77039,7 +77040,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="363" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" s="3" t="s">
         <v>1642</v>
       </c>
@@ -77083,7 +77084,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="364" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" s="3" t="s">
         <v>1646</v>
       </c>
@@ -77127,7 +77128,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="365" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" s="3" t="s">
         <v>1650</v>
       </c>
@@ -77171,7 +77172,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="366" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="s">
         <v>1654</v>
       </c>
@@ -77215,7 +77216,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="367" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="s">
         <v>1658</v>
       </c>
@@ -77259,7 +77260,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="368" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="s">
         <v>1662</v>
       </c>
@@ -77303,7 +77304,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="s">
         <v>1666</v>
       </c>
@@ -77347,7 +77348,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" s="3" t="s">
         <v>1670</v>
       </c>
@@ -77391,7 +77392,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="s">
         <v>1674</v>
       </c>
@@ -77435,7 +77436,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" s="3" t="s">
         <v>1678</v>
       </c>
@@ -77479,7 +77480,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
         <v>1684</v>
       </c>
@@ -77523,7 +77524,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="4" t="s">
         <v>1690</v>
       </c>
@@ -77567,7 +77568,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="s">
         <v>1694</v>
       </c>
@@ -77611,7 +77612,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="s">
         <v>1700</v>
       </c>
@@ -77655,7 +77656,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
         <v>1706</v>
       </c>
@@ -77699,7 +77700,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" s="3" t="s">
         <v>1710</v>
       </c>
@@ -77743,7 +77744,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
         <v>1713</v>
       </c>
@@ -77787,7 +77788,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="s">
         <v>1717</v>
       </c>
@@ -77831,7 +77832,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
         <v>1721</v>
       </c>
@@ -77875,7 +77876,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" s="3" t="s">
         <v>1725</v>
       </c>
@@ -77919,7 +77920,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
         <v>1732</v>
       </c>
@@ -77963,7 +77964,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" s="3" t="s">
         <v>1735</v>
       </c>
@@ -78007,7 +78008,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="s">
         <v>1738</v>
       </c>
@@ -78051,7 +78052,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="s">
         <v>1741</v>
       </c>
@@ -78095,7 +78096,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
         <v>1744</v>
       </c>
@@ -78139,7 +78140,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" s="3" t="s">
         <v>1748</v>
       </c>
@@ -78183,7 +78184,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" s="27" t="s">
         <v>1751</v>
       </c>
@@ -78227,7 +78228,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" s="3" t="s">
         <v>1754</v>
       </c>
@@ -78271,7 +78272,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" s="3" t="s">
         <v>1758</v>
       </c>
@@ -78315,7 +78316,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" s="3" t="s">
         <v>1762</v>
       </c>
@@ -78359,7 +78360,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="393" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
         <v>1769</v>
       </c>
@@ -78403,7 +78404,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394" s="3" t="s">
         <v>1776</v>
       </c>
@@ -78447,7 +78448,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="395" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395" s="3" t="s">
         <v>1783</v>
       </c>
@@ -78491,7 +78492,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="396" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396" s="4" t="s">
         <v>1787</v>
       </c>
@@ -78535,7 +78536,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="397" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="s">
         <v>1791</v>
       </c>
@@ -78579,7 +78580,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="398" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" s="4" t="s">
         <v>1795</v>
       </c>
@@ -78623,7 +78624,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="399" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" s="3" t="s">
         <v>1800</v>
       </c>
@@ -78667,7 +78668,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="400" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" s="3" t="s">
         <v>1807</v>
       </c>
@@ -78711,7 +78712,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="401" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" s="3" t="s">
         <v>1810</v>
       </c>
@@ -78755,7 +78756,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="402" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" s="3" t="s">
         <v>1813</v>
       </c>
@@ -78799,7 +78800,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="403" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" s="3" t="s">
         <v>1816</v>
       </c>
@@ -78843,7 +78844,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="404" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" s="3" t="s">
         <v>1823</v>
       </c>
@@ -78887,7 +78888,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="405" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" s="3" t="s">
         <v>1826</v>
       </c>
@@ -78931,7 +78932,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="406" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" s="3" t="s">
         <v>1830</v>
       </c>
@@ -78975,7 +78976,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="407" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" s="3" t="s">
         <v>1834</v>
       </c>
@@ -79019,7 +79020,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="408" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" s="3" t="s">
         <v>1838</v>
       </c>
@@ -79063,7 +79064,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="409" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
         <v>1842</v>
       </c>
@@ -79107,7 +79108,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="410" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" s="3" t="s">
         <v>1846</v>
       </c>
@@ -79151,7 +79152,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="411" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" s="3" t="s">
         <v>1850</v>
       </c>
@@ -79195,7 +79196,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="412" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" s="3" t="s">
         <v>1854</v>
       </c>
@@ -79239,7 +79240,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="413" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" s="3" t="s">
         <v>1858</v>
       </c>
@@ -79283,7 +79284,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="414" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" s="3" t="s">
         <v>1862</v>
       </c>
@@ -79327,7 +79328,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="415" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" s="3" t="s">
         <v>1866</v>
       </c>
@@ -79371,7 +79372,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="416" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" s="3" t="s">
         <v>1870</v>
       </c>
@@ -79415,7 +79416,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="417" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" s="3" t="s">
         <v>1874</v>
       </c>
@@ -79459,7 +79460,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="418" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" s="3" t="s">
         <v>1878</v>
       </c>
@@ -79503,7 +79504,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="419" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" s="3" t="s">
         <v>1882</v>
       </c>
@@ -79547,7 +79548,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="420" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" s="3" t="s">
         <v>1885</v>
       </c>
@@ -79591,7 +79592,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="421" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" s="3" t="s">
         <v>1889</v>
       </c>
@@ -79635,7 +79636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="422" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" s="3" t="s">
         <v>1893</v>
       </c>
@@ -79679,7 +79680,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="423" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423" s="3" t="s">
         <v>1900</v>
       </c>
@@ -79723,7 +79724,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="424" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424" s="3" t="s">
         <v>1907</v>
       </c>
@@ -79767,7 +79768,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="425" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425" s="3" t="s">
         <v>1910</v>
       </c>
@@ -79811,7 +79812,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="426" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" s="3" t="s">
         <v>1913</v>
       </c>
@@ -79855,7 +79856,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="427" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427" s="3" t="s">
         <v>1916</v>
       </c>
@@ -79899,7 +79900,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="428" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" s="3" t="s">
         <v>1919</v>
       </c>
@@ -79943,7 +79944,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="429" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" s="3" t="s">
         <v>1922</v>
       </c>
@@ -79987,7 +79988,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="430" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430" s="3" t="s">
         <v>1929</v>
       </c>
@@ -80031,7 +80032,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="431" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431" s="3" t="s">
         <v>1932</v>
       </c>
@@ -80075,7 +80076,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="432" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432" s="3" t="s">
         <v>1935</v>
       </c>
@@ -80119,7 +80120,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="433" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433" s="3" t="s">
         <v>1938</v>
       </c>
@@ -80163,7 +80164,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="434" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434" s="3" t="s">
         <v>1941</v>
       </c>
@@ -80207,7 +80208,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="435" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" s="3" t="s">
         <v>1944</v>
       </c>
@@ -80251,7 +80252,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="436" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" s="3" t="s">
         <v>1947</v>
       </c>
@@ -80295,7 +80296,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="437" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" s="3" t="s">
         <v>1950</v>
       </c>
@@ -80339,7 +80340,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="438" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438" s="27" t="s">
         <v>1953</v>
       </c>
@@ -80383,7 +80384,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="439" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A439" s="3" t="s">
         <v>1960</v>
       </c>
@@ -80427,7 +80428,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="440" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" s="3" t="s">
         <v>1964</v>
       </c>
@@ -80471,7 +80472,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="441" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441" s="3" t="s">
         <v>1968</v>
       </c>
@@ -80515,7 +80516,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="442" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442" s="3" t="s">
         <v>1972</v>
       </c>
@@ -80559,7 +80560,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="443" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A443" s="3" t="s">
         <v>1976</v>
       </c>
@@ -80603,7 +80604,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="444" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444" s="3" t="s">
         <v>1980</v>
       </c>
@@ -80647,7 +80648,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="445" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" s="3" t="s">
         <v>1984</v>
       </c>
@@ -80691,7 +80692,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="446" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" s="3" t="s">
         <v>1988</v>
       </c>
@@ -80735,7 +80736,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="447" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447" s="3" t="s">
         <v>1992</v>
       </c>
@@ -80779,7 +80780,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="448" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" s="3" t="s">
         <v>1996</v>
       </c>
@@ -80823,7 +80824,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="449" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" s="3" t="s">
         <v>2000</v>
       </c>
@@ -80867,7 +80868,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="450" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" s="3" t="s">
         <v>2004</v>
       </c>
@@ -80911,7 +80912,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="451" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="3" t="s">
         <v>2008</v>
       </c>
@@ -80955,7 +80956,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="452" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="3" t="s">
         <v>2011</v>
       </c>
@@ -80999,7 +81000,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="453" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" s="3" t="s">
         <v>2014</v>
       </c>
@@ -81043,7 +81044,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="454" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" s="3" t="s">
         <v>2018</v>
       </c>
@@ -81087,7 +81088,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="455" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" s="3" t="s">
         <v>2022</v>
       </c>
@@ -81131,7 +81132,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="456" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" s="3" t="s">
         <v>2026</v>
       </c>
@@ -81175,7 +81176,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="457" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" s="3" t="s">
         <v>2030</v>
       </c>
@@ -81219,7 +81220,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="458" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458" s="3" t="s">
         <v>2034</v>
       </c>
@@ -81263,7 +81264,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="459" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" s="3" t="s">
         <v>2037</v>
       </c>
@@ -81307,7 +81308,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="460" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" s="3" t="s">
         <v>2041</v>
       </c>
@@ -81351,7 +81352,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="461" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="3" t="s">
         <v>2045</v>
       </c>
@@ -81395,7 +81396,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="462" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462" s="3" t="s">
         <v>2049</v>
       </c>
@@ -81439,7 +81440,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="463" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" s="3" t="s">
         <v>2053</v>
       </c>
@@ -81483,7 +81484,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="464" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" s="3" t="s">
         <v>2057</v>
       </c>
@@ -81527,7 +81528,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="465" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" s="3" t="s">
         <v>2061</v>
       </c>
@@ -81571,7 +81572,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="466" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" s="3" t="s">
         <v>2065</v>
       </c>
@@ -81615,7 +81616,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="467" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467" s="3" t="s">
         <v>2069</v>
       </c>
@@ -81659,7 +81660,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="468" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A468" s="3" t="s">
         <v>2073</v>
       </c>
@@ -81703,7 +81704,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="469" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A469" s="3" t="s">
         <v>2077</v>
       </c>
@@ -81747,7 +81748,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="470" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A470" s="3" t="s">
         <v>2081</v>
       </c>
@@ -81791,7 +81792,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="471" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A471" s="3" t="s">
         <v>2085</v>
       </c>
@@ -81835,7 +81836,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="472" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472" s="3" t="s">
         <v>2089</v>
       </c>
@@ -81879,7 +81880,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="473" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A473" s="3" t="s">
         <v>2093</v>
       </c>
@@ -81923,7 +81924,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="474" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" s="3" t="s">
         <v>2097</v>
       </c>
@@ -81967,7 +81968,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="475" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475" s="3" t="s">
         <v>2100</v>
       </c>
@@ -82011,7 +82012,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="476" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" s="3" t="s">
         <v>2104</v>
       </c>
@@ -82055,7 +82056,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="477" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" s="3" t="s">
         <v>2107</v>
       </c>
@@ -82099,7 +82100,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="478" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478" s="3" t="s">
         <v>2111</v>
       </c>
@@ -82143,7 +82144,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="479" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A479" s="3" t="s">
         <v>2115</v>
       </c>
@@ -82187,7 +82188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="480" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480" s="3" t="s">
         <v>2119</v>
       </c>
@@ -82231,7 +82232,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="481" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" s="3" t="s">
         <v>2123</v>
       </c>
@@ -82275,7 +82276,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="482" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A482" s="3" t="s">
         <v>2126</v>
       </c>
@@ -82319,7 +82320,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="483" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" s="3" t="s">
         <v>2129</v>
       </c>
@@ -82363,7 +82364,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="484" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484" s="3" t="s">
         <v>2132</v>
       </c>
@@ -82407,7 +82408,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="485" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A485" s="3" t="s">
         <v>2135</v>
       </c>
@@ -82451,7 +82452,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="486" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A486" s="3" t="s">
         <v>2138</v>
       </c>
@@ -82495,7 +82496,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="487" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A487" s="3" t="s">
         <v>2142</v>
       </c>
@@ -82539,7 +82540,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="488" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A488" s="3" t="s">
         <v>2145</v>
       </c>
@@ -82583,7 +82584,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="489" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489" s="3" t="s">
         <v>2149</v>
       </c>
@@ -82627,7 +82628,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="490" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" s="3" t="s">
         <v>2153</v>
       </c>
@@ -82671,7 +82672,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="491" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" s="3" t="s">
         <v>2156</v>
       </c>
@@ -82715,7 +82716,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="492" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" s="3" t="s">
         <v>2160</v>
       </c>
@@ -82759,7 +82760,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="493" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" s="3" t="s">
         <v>2164</v>
       </c>
@@ -82803,7 +82804,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="494" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A494" s="3" t="s">
         <v>2167</v>
       </c>
@@ -82847,7 +82848,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="495" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" s="3" t="s">
         <v>2171</v>
       </c>
@@ -82891,7 +82892,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="496" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" s="3" t="s">
         <v>2175</v>
       </c>
@@ -82935,7 +82936,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="497" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" s="3" t="s">
         <v>2179</v>
       </c>
@@ -82979,7 +82980,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="498" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A498" s="3" t="s">
         <v>2183</v>
       </c>
@@ -83023,7 +83024,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="499" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A499" s="3" t="s">
         <v>2187</v>
       </c>
@@ -83067,7 +83068,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="500" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A500" s="3" t="s">
         <v>2191</v>
       </c>
@@ -83111,7 +83112,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="501" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A501" s="3" t="s">
         <v>2195</v>
       </c>
@@ -83155,7 +83156,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="502" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A502" s="3" t="s">
         <v>2199</v>
       </c>
@@ -83199,7 +83200,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="503" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A503" s="3" t="s">
         <v>2203</v>
       </c>
@@ -83243,7 +83244,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="504" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" s="3" t="s">
         <v>2207</v>
       </c>
@@ -83287,7 +83288,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="505" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A505" s="3" t="s">
         <v>2211</v>
       </c>
@@ -83331,7 +83332,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="506" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A506" s="3" t="s">
         <v>2215</v>
       </c>
@@ -83375,7 +83376,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="507" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A507" s="3" t="s">
         <v>2219</v>
       </c>
@@ -83419,7 +83420,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="508" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A508" s="3" t="s">
         <v>2223</v>
       </c>
@@ -83463,7 +83464,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="509" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A509" s="3" t="s">
         <v>2227</v>
       </c>
@@ -83507,7 +83508,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="510" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A510" s="3" t="s">
         <v>2231</v>
       </c>
@@ -83551,7 +83552,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="511" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A511" s="3" t="s">
         <v>2234</v>
       </c>
@@ -83595,7 +83596,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="512" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A512" s="3" t="s">
         <v>2237</v>
       </c>
@@ -83639,7 +83640,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="513" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A513" s="3" t="s">
         <v>2240</v>
       </c>
@@ -83683,7 +83684,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="514" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A514" s="3" t="s">
         <v>2243</v>
       </c>
@@ -83727,7 +83728,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="515" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A515" s="3" t="s">
         <v>2247</v>
       </c>
@@ -83771,7 +83772,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="516" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A516" s="3" t="s">
         <v>2254</v>
       </c>
@@ -83815,7 +83816,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="517" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A517" s="3" t="s">
         <v>2257</v>
       </c>
@@ -83859,7 +83860,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="518" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A518" s="3" t="s">
         <v>2261</v>
       </c>
@@ -83903,7 +83904,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="519" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A519" s="3" t="s">
         <v>2265</v>
       </c>
@@ -83947,7 +83948,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="520" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A520" s="3" t="s">
         <v>2269</v>
       </c>
@@ -83991,7 +83992,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="521" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A521" s="3" t="s">
         <v>2273</v>
       </c>
@@ -84035,7 +84036,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="522" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A522" s="3" t="s">
         <v>2277</v>
       </c>
@@ -84079,7 +84080,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="523" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A523" s="3" t="s">
         <v>2281</v>
       </c>
@@ -84124,7 +84125,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N523" xr:uid="{5D116E73-55E3-504B-8741-15E6858173B5}"/>
+  <autoFilter ref="A1:N523" xr:uid="{5D116E73-55E3-504B-8741-15E6858173B5}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Aulonocara baenschi"/>
+        <filter val="Aulonocara blue chilumba"/>
+        <filter val="Aulonocara gold"/>
+        <filter val="Aulonocara minutus"/>
+        <filter val="Aulonocara Nkhata &quot;yellow head&quot; chitende"/>
+        <filter val="Aulonocara steveni"/>
+        <filter val="Aulonocara stuartgranti"/>
+        <filter val="Aulonocara stuartgranti maisoni"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="Q3:Q11"/>
   </mergeCells>

</xml_diff>

<commit_message>
implemented a pipeline to download new GVCF files and run joint genotyping with GATK GenomicsDBImport and GenotypeGVCFs
</commit_message>
<xml_diff>
--- a/cichlid_sr_sequencing/SampleDatabase.xlsx
+++ b/cichlid_sr_sequencing/SampleDatabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmnike/Desktop/VCF_Excel_Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmnike/CichlidSRSequencing/cichlid_sr_sequencing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DD7C22-A825-624A-8C8E-E5CE2DA0D0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276B489B-C96A-9144-8C8E-0E74ADF4F7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35740" yWindow="1080" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleDatabase_Fixed_Ecogroups" sheetId="1" r:id="rId1"/>
@@ -7089,7 +7089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7141,7 +7141,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60799,8 +60798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D116E73-55E3-504B-8741-15E6858173B5}">
   <dimension ref="A1:U523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A479" zoomScale="114" workbookViewId="0">
-      <selection activeCell="K501" sqref="K501"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -71093,90 +71092,90 @@
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A228" s="29" t="s">
+      <c r="A228" s="3" t="s">
         <v>1059</v>
       </c>
-      <c r="B228" s="29" t="s">
+      <c r="B228" s="3" t="s">
         <v>1060</v>
       </c>
-      <c r="C228" s="29">
+      <c r="C228" s="3">
         <v>200</v>
       </c>
-      <c r="D228" s="29">
+      <c r="D228" s="3">
         <v>3815601600</v>
       </c>
-      <c r="E228" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F228" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G228" s="29">
+      <c r="E228" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F228" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G228" s="3">
         <v>6526433</v>
       </c>
-      <c r="H228" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I228" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="J228" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K228" s="29" t="s">
+      <c r="H228" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I228" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J228" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K228" s="3" t="s">
         <v>1061</v>
       </c>
-      <c r="L228" s="29" t="s">
+      <c r="L228" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="M228" s="29" t="s">
+      <c r="M228" s="3" t="s">
         <v>2285</v>
       </c>
-      <c r="N228" s="29" t="s">
+      <c r="N228" s="3" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A229" s="29" t="s">
+      <c r="A229" s="3" t="s">
         <v>1066</v>
       </c>
-      <c r="B229" s="29" t="s">
+      <c r="B229" s="3" t="s">
         <v>1067</v>
       </c>
-      <c r="C229" s="29">
+      <c r="C229" s="3">
         <v>200</v>
       </c>
-      <c r="D229" s="29">
+      <c r="D229" s="3">
         <v>21054829822</v>
       </c>
-      <c r="E229" s="29" t="s">
+      <c r="E229" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="F229" s="29" t="s">
+      <c r="F229" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="G229" s="29" t="s">
+      <c r="G229" s="3" t="s">
         <v>1068</v>
       </c>
-      <c r="H229" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I229" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="J229" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K229" s="29" t="s">
+      <c r="H229" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I229" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J229" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K229" s="3" t="s">
         <v>1069</v>
       </c>
-      <c r="L229" s="29" t="s">
+      <c r="L229" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="M229" s="29" t="s">
+      <c r="M229" s="3" t="s">
         <v>2285</v>
       </c>
-      <c r="N229" s="29" t="s">
+      <c r="N229" s="3" t="s">
         <v>181</v>
       </c>
     </row>

</xml_diff>